<commit_message>
Atualização do arquivo das tabelas
</commit_message>
<xml_diff>
--- a/tabelas/direcao_saida.xlsx
+++ b/tabelas/direcao_saida.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,23 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>id_direcao_saida</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>direcao_saida</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+        <v>43409</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>Carga Piezométrica</t>
         </is>
@@ -452,109 +460,129 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Cota NA</t>
+        <v>48808</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cota Piezométrica</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Cota Piezométrica</t>
+        <v>7271</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cota do NA</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cota do NA</t>
+        <v>23375</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Deslocamento Longitudinal (X)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Deslocamento Longitudinal (X)</t>
+        <v>22596</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Deslocamento Transversal (Y)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Deslocamento Transversal (Y)</t>
+        <v>45750</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Deslocamento da Estaca Dir(-)/Esq(+)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Deslocamento da Estaca Dir(-)/Esq(+)</t>
+        <v>20547</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Deslocamento do Afastamento Mont(-)/Jus(+)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Deslocamento do Afastamento Mont(-)/Jus(+)</t>
+        <v>28397</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Leitura</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Leitura</t>
+        <v>33011</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Recalque</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Recalque</t>
+        <v>23084</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Recalque (Z)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Recalque (Z)</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
+        <v>33897</v>
+      </c>
+      <c r="B12" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Vazão</t>
         </is>

</xml_diff>